<commit_message>
zomato with data driven menu
</commit_message>
<xml_diff>
--- a/inputFile/InputFile.xlsx
+++ b/inputFile/InputFile.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathishkumar\PycharmProjects\WeekdayPython\inputFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650C759-CC25-4734-A5AD-0292F0087C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECE8931-0DA1-42D0-A017-CAD99B25A916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Veg" sheetId="2" r:id="rId2"/>
+    <sheet name="NonVeg" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>username</t>
   </si>
@@ -80,14 +81,76 @@
   </si>
   <si>
     <t>institute</t>
+  </si>
+  <si>
+    <t>A2B</t>
+  </si>
+  <si>
+    <t>SRR</t>
+  </si>
+  <si>
+    <t>SRV</t>
+  </si>
+  <si>
+    <t>Idly-8</t>
+  </si>
+  <si>
+    <t>Dosa-30</t>
+  </si>
+  <si>
+    <t>Vada-45</t>
+  </si>
+  <si>
+    <t>Poori-60</t>
+  </si>
+  <si>
+    <t>MasalDosa -75</t>
+  </si>
+  <si>
+    <t>Idly-9</t>
+  </si>
+  <si>
+    <t>Dosa-40</t>
+  </si>
+  <si>
+    <t>Vada-5</t>
+  </si>
+  <si>
+    <t>Poori-20</t>
+  </si>
+  <si>
+    <t>MasalDosa -55</t>
+  </si>
+  <si>
+    <t>Idly-5</t>
+  </si>
+  <si>
+    <t>Dosa-31</t>
+  </si>
+  <si>
+    <t>Vada-40</t>
+  </si>
+  <si>
+    <t>Poori-10</t>
+  </si>
+  <si>
+    <t>MasalDosa -65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -115,8 +178,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -481,6 +545,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91903CED-57A9-462D-970E-7DC29F302CB5}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FF4882-87A9-4CDD-B999-F813540E2878}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>